<commit_message>
chore: remove space on excel file for vehicles info
</commit_message>
<xml_diff>
--- a/scripts/to_csv/vehicles_info.xlsx
+++ b/scripts/to_csv/vehicles_info.xlsx
@@ -803,7 +803,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="670">
   <si>
     <t>version_name</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -2977,10 +2977,6 @@
   </si>
   <si>
     <t>DENZA Z9 GT</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">DENZA Z9 GT </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3573,8 +3569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J115" sqref="J115"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -3816,7 +3812,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="7" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>612</v>

</xml_diff>